<commit_message>
Added test cases for Search Section
9 test cases are added for Search section along with that also modified testbase setup function to launch browser based on config.properties browser
</commit_message>
<xml_diff>
--- a/QI_Assignment/src/test/resources/data/TestData.xlsx
+++ b/QI_Assignment/src/test/resources/data/TestData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QI_Assignment\QI_Assignment_DD\QI_Assignment\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Documents\GitHub\QI_InterviewAssignment\QI_Assignment\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8D473A-5F09-41C9-94C7-AEC30C60D8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F4AA07-7C4B-4B5F-90BF-65E3B6E6C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sanity" sheetId="12" r:id="rId1"/>
     <sheet name="LandingPageTest" sheetId="11" r:id="rId2"/>
+    <sheet name="SearchPageTest" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -86,13 +87,43 @@
   </si>
   <si>
     <t>automationtestbypk@gmail.com</t>
+  </si>
+  <si>
+    <t>SearchPageTest</t>
+  </si>
+  <si>
+    <t>SearchBoxPlaceHolderText</t>
+  </si>
+  <si>
+    <t>InputToTestCancelBtn</t>
+  </si>
+  <si>
+    <t>TC001_SearchPageTest</t>
+  </si>
+  <si>
+    <t>Search OneMap</t>
+  </si>
+  <si>
+    <t>Text for Cancel Button</t>
+  </si>
+  <si>
+    <t>InputForTestSearch</t>
+  </si>
+  <si>
+    <t>DepartureTime</t>
+  </si>
+  <si>
+    <t>12:30 a.m.</t>
+  </si>
+  <si>
+    <t>Bayfront MRT Station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +149,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -165,6 +203,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0077092-9009-49D9-BD6B-8FE867BDBBFE}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -489,6 +531,20 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -571,4 +627,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C6E9F2-A30F-40AD-84E5-1F0D3E1DBB9D}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>